<commit_message>
Tests on home computer
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DITF.project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DITF.project\acc-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7218B42B-B8E8-441D-9967-CB1AD909EC70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBDFBAE-F31B-45E3-B2CA-6BDDE2ABA372}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" activeTab="3" xr2:uid="{838B111C-B0DA-4F59-BCE8-B8724B0C9FA4}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="52">
   <si>
     <t>0S</t>
   </si>
@@ -684,6 +684,270 @@
         <scheme val="minor"/>
       </rPr>
       <t>: 3  000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OS: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Windows 10, gcc version 13.2.0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+CPU: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Intel(R) Core(TM) i7 CPU 860  @ 2.80GHz   2.93 GHz</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+GPU:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> NVIDIA GeForce GTX 1050, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Test size:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 5  000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OS: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Windows 10, gcc version 13.2.0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+CPU:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Intel(R) Core(TM) i7 CPU 860  @ 2.80GHz   2.93 GHz</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+GPU: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NVIDIA GeForce GTX 1050, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Test size: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 000 000 000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OS: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Windows 10, gcc version 13.2.0,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+CPU:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Intel(R) Core(TM) i7 CPU 860  @ 2.80GHz   2.93 GHz</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+GPU: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NVIDIA GeForce GTX 1050, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Test size: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2 000 000 000</t>
     </r>
   </si>
 </sst>
@@ -1131,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B2F90D-FE91-46B6-9FE4-069E95EAE76E}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,21 +2355,437 @@
       </c>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
+    <row r="37" spans="1:13" s="2" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1937</v>
+      </c>
+      <c r="C38">
+        <v>3942</v>
+      </c>
+      <c r="D38">
+        <v>1428</v>
+      </c>
+      <c r="E38">
+        <v>1467</v>
+      </c>
+      <c r="F38">
+        <v>1419</v>
+      </c>
+      <c r="G38">
+        <v>1495</v>
+      </c>
+      <c r="H38">
+        <v>1559</v>
+      </c>
+      <c r="I38">
+        <v>954</v>
+      </c>
+      <c r="J38">
+        <v>916</v>
+      </c>
+      <c r="K38">
+        <v>923</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
+      <c r="B39">
+        <v>1461</v>
+      </c>
+      <c r="C39">
+        <v>3879</v>
+      </c>
+      <c r="D39">
+        <v>1473</v>
+      </c>
+      <c r="E39">
+        <v>1431</v>
+      </c>
+      <c r="F39">
+        <v>1391</v>
+      </c>
+      <c r="G39">
+        <v>1497</v>
+      </c>
+      <c r="H39">
+        <v>1595</v>
+      </c>
+      <c r="I39">
+        <v>909</v>
+      </c>
+      <c r="J39">
+        <v>956</v>
+      </c>
+      <c r="K39">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1474</v>
+      </c>
+      <c r="C40">
+        <v>3928</v>
+      </c>
+      <c r="D40">
+        <v>1453</v>
+      </c>
+      <c r="E40">
+        <v>1432</v>
+      </c>
+      <c r="F40">
+        <v>1419</v>
+      </c>
+      <c r="G40">
+        <v>1485</v>
+      </c>
+      <c r="H40">
+        <v>1636</v>
+      </c>
+      <c r="I40">
+        <v>944</v>
+      </c>
+      <c r="J40">
+        <v>931</v>
+      </c>
+      <c r="K40">
+        <v>907</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="K41" s="7"/>
+      <c r="B41">
+        <v>1454</v>
+      </c>
+      <c r="C41">
+        <v>3927</v>
+      </c>
+      <c r="D41">
+        <v>1437</v>
+      </c>
+      <c r="E41">
+        <v>1426</v>
+      </c>
+      <c r="F41">
+        <v>1399</v>
+      </c>
+      <c r="G41">
+        <v>1488</v>
+      </c>
+      <c r="H41">
+        <v>1567</v>
+      </c>
+      <c r="I41">
+        <v>938</v>
+      </c>
+      <c r="J41">
+        <v>908</v>
+      </c>
+      <c r="K41">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>1452</v>
+      </c>
+      <c r="C42">
+        <v>3930</v>
+      </c>
+      <c r="D42">
+        <v>1418</v>
+      </c>
+      <c r="E42">
+        <v>1433</v>
+      </c>
+      <c r="F42">
+        <v>1400</v>
+      </c>
+      <c r="G42">
+        <v>1520</v>
+      </c>
+      <c r="H42">
+        <v>1707</v>
+      </c>
+      <c r="I42">
+        <v>920</v>
+      </c>
+      <c r="J42">
+        <v>916</v>
+      </c>
+      <c r="K42">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>1413</v>
+      </c>
+      <c r="C43">
+        <v>3902</v>
+      </c>
+      <c r="D43">
+        <v>1462</v>
+      </c>
+      <c r="E43">
+        <v>1438</v>
+      </c>
+      <c r="F43">
+        <v>1408</v>
+      </c>
+      <c r="G43">
+        <v>1496</v>
+      </c>
+      <c r="H43">
+        <v>1583</v>
+      </c>
+      <c r="I43">
+        <v>923</v>
+      </c>
+      <c r="J43">
+        <v>940</v>
+      </c>
+      <c r="K43">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1422</v>
+      </c>
+      <c r="C44">
+        <v>3911</v>
+      </c>
+      <c r="D44">
+        <v>1481</v>
+      </c>
+      <c r="E44">
+        <v>1432</v>
+      </c>
+      <c r="F44">
+        <v>1413</v>
+      </c>
+      <c r="G44">
+        <v>1494</v>
+      </c>
+      <c r="H44">
+        <v>1553</v>
+      </c>
+      <c r="I44">
+        <v>919</v>
+      </c>
+      <c r="J44">
+        <v>928</v>
+      </c>
+      <c r="K44">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>1449</v>
+      </c>
+      <c r="C45">
+        <v>3924</v>
+      </c>
+      <c r="D45">
+        <v>1474</v>
+      </c>
+      <c r="E45">
+        <v>1417</v>
+      </c>
+      <c r="F45">
+        <v>1414</v>
+      </c>
+      <c r="G45">
+        <v>1496</v>
+      </c>
+      <c r="H45">
+        <v>1692</v>
+      </c>
+      <c r="I45">
+        <v>904</v>
+      </c>
+      <c r="J45">
+        <v>949</v>
+      </c>
+      <c r="K45">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>1423</v>
+      </c>
+      <c r="C46">
+        <v>3947</v>
+      </c>
+      <c r="D46">
+        <v>1477</v>
+      </c>
+      <c r="E46">
+        <v>1464</v>
+      </c>
+      <c r="F46">
+        <v>1404</v>
+      </c>
+      <c r="G46">
+        <v>1509</v>
+      </c>
+      <c r="H46">
+        <v>1589</v>
+      </c>
+      <c r="I46">
+        <v>902</v>
+      </c>
+      <c r="J46">
+        <v>929</v>
+      </c>
+      <c r="K46">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>1432</v>
+      </c>
+      <c r="C47">
+        <v>3910</v>
+      </c>
+      <c r="D47">
+        <v>1450</v>
+      </c>
+      <c r="E47">
+        <v>1455</v>
+      </c>
+      <c r="F47">
+        <v>1397</v>
+      </c>
+      <c r="G47">
+        <v>1501</v>
+      </c>
+      <c r="H47">
+        <v>1590</v>
+      </c>
+      <c r="I47">
+        <v>910</v>
+      </c>
+      <c r="J47">
+        <v>906</v>
+      </c>
+      <c r="K47">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3">
+        <f>MIN(B38:B47)</f>
+        <v>1413</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" ref="C48:K48" si="4">MIN(C38:C47)</f>
+        <v>3879</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="4"/>
+        <v>1418</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="4"/>
+        <v>1417</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="4"/>
+        <v>1391</v>
+      </c>
+      <c r="G48" s="3">
+        <f t="shared" si="4"/>
+        <v>1485</v>
+      </c>
+      <c r="H48" s="3">
+        <f t="shared" si="4"/>
+        <v>1553</v>
+      </c>
+      <c r="I48" s="3">
+        <f t="shared" si="4"/>
+        <v>902</v>
+      </c>
+      <c r="J48" s="3">
+        <f t="shared" si="4"/>
+        <v>906</v>
+      </c>
+      <c r="K48" s="3">
+        <f t="shared" si="4"/>
+        <v>902</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="12">
+        <f>B48/$B$48*100</f>
+        <v>100</v>
+      </c>
+      <c r="C49" s="11">
+        <f t="shared" ref="C49:K49" si="5">C48/$B$48*100</f>
+        <v>274.52229299363057</v>
+      </c>
+      <c r="D49" s="11">
+        <f t="shared" si="5"/>
+        <v>100.35385704175512</v>
+      </c>
+      <c r="E49" s="11">
+        <f t="shared" si="5"/>
+        <v>100.28308563340411</v>
+      </c>
+      <c r="F49" s="11">
+        <f t="shared" si="5"/>
+        <v>98.443029016277421</v>
+      </c>
+      <c r="G49" s="11">
+        <f t="shared" si="5"/>
+        <v>105.09554140127389</v>
+      </c>
+      <c r="H49" s="11">
+        <f t="shared" si="5"/>
+        <v>109.90799716914366</v>
+      </c>
+      <c r="I49" s="11">
+        <f t="shared" si="5"/>
+        <v>63.83581033262562</v>
+      </c>
+      <c r="J49" s="11">
+        <f t="shared" si="5"/>
+        <v>64.118895966029726</v>
+      </c>
+      <c r="K49" s="11">
+        <f t="shared" si="5"/>
+        <v>63.83581033262562</v>
+      </c>
+      <c r="M49" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A11:K11"/>
     <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A37:K37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2114,10 +2794,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE63084B-FAB7-42C6-903C-DEC7AAD98ECD}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="T53" sqref="T53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2922,7 +3602,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>924</v>
       </c>
@@ -2954,7 +3634,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>925</v>
       </c>
@@ -2986,7 +3666,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -3031,7 +3711,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>10</v>
       </c>
@@ -3077,21 +3757,440 @@
       </c>
       <c r="M36" s="4"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="K41" s="7"/>
+    <row r="37" spans="1:14" s="2" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>11360</v>
+      </c>
+      <c r="C38">
+        <v>5640</v>
+      </c>
+      <c r="D38">
+        <v>3042</v>
+      </c>
+      <c r="E38">
+        <v>2900</v>
+      </c>
+      <c r="F38">
+        <v>3323</v>
+      </c>
+      <c r="G38">
+        <v>3300</v>
+      </c>
+      <c r="H38">
+        <v>3606</v>
+      </c>
+      <c r="I38">
+        <v>2901</v>
+      </c>
+      <c r="J38">
+        <v>3021</v>
+      </c>
+      <c r="K38">
+        <v>3054</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>25208</v>
+      </c>
+      <c r="C39">
+        <v>3521</v>
+      </c>
+      <c r="D39" s="7">
+        <v>1952</v>
+      </c>
+      <c r="E39">
+        <v>1992</v>
+      </c>
+      <c r="F39">
+        <v>2320</v>
+      </c>
+      <c r="G39">
+        <v>2391</v>
+      </c>
+      <c r="H39">
+        <v>2549</v>
+      </c>
+      <c r="I39" s="7">
+        <v>1879</v>
+      </c>
+      <c r="J39">
+        <v>1845</v>
+      </c>
+      <c r="K39" s="7">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>3540</v>
+      </c>
+      <c r="C40">
+        <v>3780</v>
+      </c>
+      <c r="D40">
+        <v>1943</v>
+      </c>
+      <c r="E40">
+        <v>1960</v>
+      </c>
+      <c r="F40">
+        <v>2325</v>
+      </c>
+      <c r="G40">
+        <v>2370</v>
+      </c>
+      <c r="H40">
+        <v>2574</v>
+      </c>
+      <c r="I40">
+        <v>1890</v>
+      </c>
+      <c r="J40">
+        <v>1858</v>
+      </c>
+      <c r="K40">
+        <v>1853</v>
+      </c>
+      <c r="N40" s="7"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>2589</v>
+      </c>
+      <c r="C41">
+        <v>3689</v>
+      </c>
+      <c r="D41">
+        <v>1944</v>
+      </c>
+      <c r="E41">
+        <v>1947</v>
+      </c>
+      <c r="F41">
+        <v>2321</v>
+      </c>
+      <c r="G41">
+        <v>2454</v>
+      </c>
+      <c r="H41">
+        <v>2579</v>
+      </c>
+      <c r="I41">
+        <v>1878</v>
+      </c>
+      <c r="J41">
+        <v>1833</v>
+      </c>
+      <c r="K41">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>2337</v>
+      </c>
+      <c r="C42">
+        <v>3492</v>
+      </c>
+      <c r="D42">
+        <v>1959</v>
+      </c>
+      <c r="E42">
+        <v>1948</v>
+      </c>
+      <c r="F42">
+        <v>2374</v>
+      </c>
+      <c r="G42">
+        <v>2696</v>
+      </c>
+      <c r="H42">
+        <v>2547</v>
+      </c>
+      <c r="I42">
+        <v>1894</v>
+      </c>
+      <c r="J42">
+        <v>1936</v>
+      </c>
+      <c r="K42">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>2348</v>
+      </c>
+      <c r="C43">
+        <v>3507</v>
+      </c>
+      <c r="D43">
+        <v>1943</v>
+      </c>
+      <c r="E43">
+        <v>1957</v>
+      </c>
+      <c r="F43">
+        <v>2314</v>
+      </c>
+      <c r="G43">
+        <v>2535</v>
+      </c>
+      <c r="H43">
+        <v>2540</v>
+      </c>
+      <c r="I43">
+        <v>1906</v>
+      </c>
+      <c r="J43">
+        <v>1831</v>
+      </c>
+      <c r="K43">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>2380</v>
+      </c>
+      <c r="C44">
+        <v>3519</v>
+      </c>
+      <c r="D44">
+        <v>1930</v>
+      </c>
+      <c r="E44">
+        <v>1932</v>
+      </c>
+      <c r="F44">
+        <v>2306</v>
+      </c>
+      <c r="G44">
+        <v>2460</v>
+      </c>
+      <c r="H44">
+        <v>2557</v>
+      </c>
+      <c r="I44">
+        <v>1869</v>
+      </c>
+      <c r="J44">
+        <v>1828</v>
+      </c>
+      <c r="K44">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>2376</v>
+      </c>
+      <c r="C45">
+        <v>3474</v>
+      </c>
+      <c r="D45">
+        <v>1932</v>
+      </c>
+      <c r="E45">
+        <v>1943</v>
+      </c>
+      <c r="F45">
+        <v>2327</v>
+      </c>
+      <c r="G45">
+        <v>2395</v>
+      </c>
+      <c r="H45">
+        <v>2578</v>
+      </c>
+      <c r="I45">
+        <v>1875</v>
+      </c>
+      <c r="J45">
+        <v>1822</v>
+      </c>
+      <c r="K45">
+        <v>1862</v>
+      </c>
+      <c r="N45" s="7"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>2325</v>
+      </c>
+      <c r="C46">
+        <v>3474</v>
+      </c>
+      <c r="D46">
+        <v>1937</v>
+      </c>
+      <c r="E46">
+        <v>1954</v>
+      </c>
+      <c r="F46">
+        <v>2331</v>
+      </c>
+      <c r="G46">
+        <v>2371</v>
+      </c>
+      <c r="H46">
+        <v>2644</v>
+      </c>
+      <c r="I46">
+        <v>1928</v>
+      </c>
+      <c r="J46">
+        <v>1812</v>
+      </c>
+      <c r="K46">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>2342</v>
+      </c>
+      <c r="C47">
+        <v>3473</v>
+      </c>
+      <c r="D47">
+        <v>1934</v>
+      </c>
+      <c r="E47">
+        <v>2015</v>
+      </c>
+      <c r="F47">
+        <v>2329</v>
+      </c>
+      <c r="G47">
+        <v>2371</v>
+      </c>
+      <c r="H47">
+        <v>2591</v>
+      </c>
+      <c r="I47">
+        <v>1895</v>
+      </c>
+      <c r="J47">
+        <v>1799</v>
+      </c>
+      <c r="K47">
+        <v>1832</v>
+      </c>
+      <c r="N47" s="7"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3">
+        <f>MIN(B38:B47)</f>
+        <v>2325</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" ref="C48:K48" si="4">MIN(C38:C47)</f>
+        <v>3473</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="4"/>
+        <v>1930</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="4"/>
+        <v>1932</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="4"/>
+        <v>2306</v>
+      </c>
+      <c r="G48" s="3">
+        <f t="shared" si="4"/>
+        <v>2370</v>
+      </c>
+      <c r="H48" s="3">
+        <f t="shared" si="4"/>
+        <v>2540</v>
+      </c>
+      <c r="I48" s="3">
+        <f t="shared" si="4"/>
+        <v>1869</v>
+      </c>
+      <c r="J48" s="3">
+        <f t="shared" si="4"/>
+        <v>1799</v>
+      </c>
+      <c r="K48" s="3">
+        <f t="shared" si="4"/>
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="12">
+        <f>B48/$B$48*100</f>
+        <v>100</v>
+      </c>
+      <c r="C49" s="11">
+        <f t="shared" ref="C49:K49" si="5">C48/$B$48*100</f>
+        <v>149.3763440860215</v>
+      </c>
+      <c r="D49" s="11">
+        <f t="shared" si="5"/>
+        <v>83.010752688172033</v>
+      </c>
+      <c r="E49" s="11">
+        <f t="shared" si="5"/>
+        <v>83.096774193548384</v>
+      </c>
+      <c r="F49" s="11">
+        <f t="shared" si="5"/>
+        <v>99.182795698924735</v>
+      </c>
+      <c r="G49" s="11">
+        <f t="shared" si="5"/>
+        <v>101.93548387096773</v>
+      </c>
+      <c r="H49" s="11">
+        <f t="shared" si="5"/>
+        <v>109.24731182795699</v>
+      </c>
+      <c r="I49" s="11">
+        <f t="shared" si="5"/>
+        <v>80.387096774193552</v>
+      </c>
+      <c r="J49" s="11">
+        <f t="shared" si="5"/>
+        <v>77.376344086021504</v>
+      </c>
+      <c r="K49" s="11">
+        <f t="shared" si="5"/>
+        <v>78.795698924731184</v>
+      </c>
+      <c r="M49" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A11:K11"/>
     <mergeCell ref="A24:K24"/>
+    <mergeCell ref="A37:K37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3100,10 +4199,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DB2D56-F0DD-4658-B708-60AFEEA597FE}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3862,7 +4961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>565</v>
       </c>
@@ -3891,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -3932,7 +5031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>10</v>
       </c>
@@ -3974,20 +5073,402 @@
       </c>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D40" s="7"/>
-      <c r="I40" s="7"/>
+    <row r="36" spans="1:13" s="2" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1823</v>
+      </c>
+      <c r="C37">
+        <v>3206</v>
+      </c>
+      <c r="D37">
+        <v>1964</v>
+      </c>
+      <c r="E37">
+        <v>2027</v>
+      </c>
+      <c r="F37">
+        <v>3185</v>
+      </c>
+      <c r="G37">
+        <v>2062</v>
+      </c>
+      <c r="H37">
+        <v>56149</v>
+      </c>
+      <c r="I37">
+        <v>59446</v>
+      </c>
+      <c r="J37">
+        <v>59232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1795</v>
+      </c>
+      <c r="C38">
+        <v>3224</v>
+      </c>
+      <c r="D38" s="7">
+        <v>1962</v>
+      </c>
+      <c r="E38">
+        <v>2034</v>
+      </c>
+      <c r="F38">
+        <v>3159</v>
+      </c>
+      <c r="G38">
+        <v>2058</v>
+      </c>
+      <c r="H38">
+        <v>55103</v>
+      </c>
+      <c r="I38" s="7">
+        <v>59248</v>
+      </c>
+      <c r="J38">
+        <v>58399</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1758</v>
+      </c>
+      <c r="C39">
+        <v>3222</v>
+      </c>
+      <c r="D39">
+        <v>1917</v>
+      </c>
+      <c r="E39">
+        <v>2035</v>
+      </c>
+      <c r="F39">
+        <v>3430</v>
+      </c>
+      <c r="G39">
+        <v>2029</v>
+      </c>
+      <c r="H39">
+        <v>54899</v>
+      </c>
+      <c r="I39">
+        <v>59197</v>
+      </c>
+      <c r="J39">
+        <v>58326</v>
+      </c>
+      <c r="M39" s="7"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1787</v>
+      </c>
+      <c r="C40">
+        <v>3205</v>
+      </c>
+      <c r="D40">
+        <v>1971</v>
+      </c>
+      <c r="E40">
+        <v>2007</v>
+      </c>
+      <c r="F40">
+        <v>3335</v>
+      </c>
+      <c r="G40">
+        <v>2082</v>
+      </c>
+      <c r="H40">
+        <v>54714</v>
+      </c>
+      <c r="I40">
+        <v>59129</v>
+      </c>
+      <c r="J40">
+        <v>58640</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>1781</v>
+      </c>
+      <c r="C41">
+        <v>3196</v>
+      </c>
+      <c r="D41">
+        <v>1909</v>
+      </c>
+      <c r="E41">
+        <v>2056</v>
+      </c>
+      <c r="F41">
+        <v>3222</v>
+      </c>
+      <c r="G41">
+        <v>2047</v>
+      </c>
+      <c r="H41">
+        <v>56293</v>
+      </c>
+      <c r="I41">
+        <v>58963</v>
+      </c>
+      <c r="J41">
+        <v>58329</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>1744</v>
+      </c>
+      <c r="C42">
+        <v>3263</v>
+      </c>
+      <c r="D42">
+        <v>1927</v>
+      </c>
+      <c r="E42">
+        <v>2008</v>
+      </c>
+      <c r="F42">
+        <v>3149</v>
+      </c>
+      <c r="G42">
+        <v>2067</v>
+      </c>
+      <c r="H42">
+        <v>55939</v>
+      </c>
+      <c r="I42">
+        <v>59205</v>
+      </c>
+      <c r="J42">
+        <v>58803</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>1789</v>
+      </c>
+      <c r="C43">
+        <v>3171</v>
+      </c>
+      <c r="D43">
+        <v>1897</v>
+      </c>
+      <c r="E43">
+        <v>2015</v>
+      </c>
+      <c r="F43">
+        <v>3160</v>
+      </c>
+      <c r="G43">
+        <v>2083</v>
+      </c>
+      <c r="H43">
+        <v>54693</v>
+      </c>
+      <c r="I43">
+        <v>59000</v>
+      </c>
+      <c r="J43">
+        <v>59353</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1765</v>
+      </c>
+      <c r="C44">
+        <v>3204</v>
+      </c>
+      <c r="D44">
+        <v>1896</v>
+      </c>
+      <c r="E44">
+        <v>1999</v>
+      </c>
+      <c r="F44">
+        <v>3141</v>
+      </c>
+      <c r="G44">
+        <v>2092</v>
+      </c>
+      <c r="H44">
+        <v>54801</v>
+      </c>
+      <c r="I44">
+        <v>59003</v>
+      </c>
+      <c r="J44">
+        <v>58851</v>
+      </c>
+      <c r="M44" s="7"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>1873</v>
+      </c>
+      <c r="C45">
+        <v>3276</v>
+      </c>
+      <c r="D45">
+        <v>1964</v>
+      </c>
+      <c r="E45">
+        <v>2095</v>
+      </c>
+      <c r="F45">
+        <v>3232</v>
+      </c>
+      <c r="G45">
+        <v>2039</v>
+      </c>
+      <c r="H45">
+        <v>54687</v>
+      </c>
+      <c r="I45">
+        <v>58975</v>
+      </c>
+      <c r="J45">
+        <v>59518</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>1833</v>
+      </c>
+      <c r="C46">
+        <v>3172</v>
+      </c>
+      <c r="D46">
+        <v>1940</v>
+      </c>
+      <c r="E46">
+        <v>2010</v>
+      </c>
+      <c r="F46">
+        <v>3112</v>
+      </c>
+      <c r="G46">
+        <v>2046</v>
+      </c>
+      <c r="H46">
+        <v>54881</v>
+      </c>
+      <c r="I46">
+        <v>61046</v>
+      </c>
+      <c r="J46">
+        <v>58354</v>
+      </c>
+      <c r="M46" s="7"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3">
+        <f>MIN(B37:B46)</f>
+        <v>1744</v>
+      </c>
+      <c r="C47" s="3">
+        <f t="shared" ref="C47:J47" si="5">MIN(C37:C46)</f>
+        <v>3171</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="5"/>
+        <v>1896</v>
+      </c>
+      <c r="E47" s="3">
+        <f t="shared" si="5"/>
+        <v>1999</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" si="5"/>
+        <v>3112</v>
+      </c>
+      <c r="G47" s="3">
+        <f t="shared" si="5"/>
+        <v>2029</v>
+      </c>
+      <c r="H47" s="3">
+        <f t="shared" si="5"/>
+        <v>54687</v>
+      </c>
+      <c r="I47" s="3">
+        <f t="shared" si="5"/>
+        <v>58963</v>
+      </c>
+      <c r="J47" s="3">
+        <f t="shared" si="5"/>
+        <v>58326</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="12">
+        <f>B47/$B$47*100</f>
+        <v>100</v>
+      </c>
+      <c r="C48" s="11">
+        <f t="shared" ref="C48:J48" si="6">C47/$B$47*100</f>
+        <v>181.82339449541286</v>
+      </c>
+      <c r="D48" s="11">
+        <f t="shared" si="6"/>
+        <v>108.71559633027523</v>
+      </c>
+      <c r="E48" s="12">
+        <f>E47/E47*100</f>
+        <v>100</v>
+      </c>
+      <c r="F48" s="11">
+        <f>F47/E47*100</f>
+        <v>155.67783891945973</v>
+      </c>
+      <c r="G48" s="11">
+        <f>G47/E47*100</f>
+        <v>101.50075037518759</v>
+      </c>
+      <c r="H48" s="12">
+        <f>H47/H47*100</f>
+        <v>100</v>
+      </c>
+      <c r="I48" s="11">
+        <f>I47/H47*100</f>
+        <v>107.81904291696381</v>
+      </c>
+      <c r="J48" s="11">
+        <f>J47/H47*100</f>
+        <v>106.65423226726645</v>
+      </c>
+      <c r="L48" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A36:K36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3996,10 +5477,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2E5D4B-1130-49F0-9A3E-7567643B3432}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O54" sqref="O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4714,19 +6195,319 @@
       </c>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
+    <row r="37" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>60053</v>
+      </c>
+      <c r="C38">
+        <v>187952</v>
+      </c>
+      <c r="D38">
+        <v>55426</v>
+      </c>
+      <c r="E38">
+        <v>56866</v>
+      </c>
+      <c r="F38">
+        <v>55291</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
+      <c r="B39">
+        <v>58375</v>
+      </c>
+      <c r="C39">
+        <v>191035</v>
+      </c>
+      <c r="D39">
+        <v>55503</v>
+      </c>
+      <c r="E39">
+        <v>57299</v>
+      </c>
+      <c r="F39">
+        <v>55358</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>58780</v>
+      </c>
+      <c r="C40">
+        <v>190558</v>
+      </c>
+      <c r="D40">
+        <v>55851</v>
+      </c>
+      <c r="E40">
+        <v>58097</v>
+      </c>
+      <c r="F40">
+        <v>55472</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D41" s="7"/>
+      <c r="B41">
+        <v>58723</v>
+      </c>
+      <c r="C41">
+        <v>190146</v>
+      </c>
+      <c r="D41">
+        <v>56289</v>
+      </c>
+      <c r="E41">
+        <v>58231</v>
+      </c>
+      <c r="F41">
+        <v>55096</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>58612</v>
+      </c>
+      <c r="C42">
+        <v>189683</v>
+      </c>
+      <c r="D42">
+        <v>56127</v>
+      </c>
+      <c r="E42">
+        <v>56792</v>
+      </c>
+      <c r="F42">
+        <v>55905</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>58313</v>
+      </c>
+      <c r="C43">
+        <v>189343</v>
+      </c>
+      <c r="D43">
+        <v>55847</v>
+      </c>
+      <c r="E43">
+        <v>56767</v>
+      </c>
+      <c r="F43">
+        <v>56135</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>58094</v>
+      </c>
+      <c r="C44">
+        <v>191598</v>
+      </c>
+      <c r="D44">
+        <v>55783</v>
+      </c>
+      <c r="E44">
+        <v>56700</v>
+      </c>
+      <c r="F44">
+        <v>56390</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>57998</v>
+      </c>
+      <c r="C45">
+        <v>188361</v>
+      </c>
+      <c r="D45">
+        <v>55846</v>
+      </c>
+      <c r="E45">
+        <v>56444</v>
+      </c>
+      <c r="F45">
+        <v>55586</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>57946</v>
+      </c>
+      <c r="C46">
+        <v>187813</v>
+      </c>
+      <c r="D46">
+        <v>56011</v>
+      </c>
+      <c r="E46">
+        <v>55561</v>
+      </c>
+      <c r="F46">
+        <v>56867</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>58257</v>
+      </c>
+      <c r="C47">
+        <v>187504</v>
+      </c>
+      <c r="D47">
+        <v>55836</v>
+      </c>
+      <c r="E47">
+        <v>55720</v>
+      </c>
+      <c r="F47">
+        <v>55872</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3">
+        <f>MIN(B38:B47)</f>
+        <v>57946</v>
+      </c>
+      <c r="C48" s="3">
+        <f t="shared" ref="C48:H48" si="4">MIN(C38:C47)</f>
+        <v>187504</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="4"/>
+        <v>55426</v>
+      </c>
+      <c r="E48" s="3">
+        <f t="shared" si="4"/>
+        <v>55561</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="4"/>
+        <v>55096</v>
+      </c>
+      <c r="G48" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="12">
+        <f>B48/$B$48*100</f>
+        <v>100</v>
+      </c>
+      <c r="C49" s="11">
+        <f t="shared" ref="C49:H49" si="5">C48/$B$48*100</f>
+        <v>323.58402650743795</v>
+      </c>
+      <c r="D49" s="11">
+        <f t="shared" si="5"/>
+        <v>95.65112345977289</v>
+      </c>
+      <c r="E49" s="11">
+        <f t="shared" si="5"/>
+        <v>95.884098988713632</v>
+      </c>
+      <c r="F49" s="11">
+        <f t="shared" si="5"/>
+        <v>95.0816277223622</v>
+      </c>
+      <c r="G49" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H49" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A37:H37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>